<commit_message>
Added TC1 - TC7
</commit_message>
<xml_diff>
--- a/test-cases/test-cases.xlsx
+++ b/test-cases/test-cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -31,31 +31,130 @@
     <t xml:space="preserve">Input</t>
   </si>
   <si>
+    <t xml:space="preserve">Steps to Execute</t>
+  </si>
+  <si>
     <t xml:space="preserve">Expected Output</t>
   </si>
   <si>
-    <t xml:space="preserve">Steps to Execute</t>
-  </si>
-  <si>
     <t xml:space="preserve">TC1</t>
   </si>
   <si>
+    <t xml:space="preserve">Valet parking – 5 hours or less – upper boundary (5 hours)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Navigate to https://www.shino.de/parkcalc/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimated parking costs: $12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valet Parking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Choose a Parking Lot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system shows the parking duration correctly as</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arbitrary date and time that is not in the past</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Input entry date and time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0 Days, 5 Hours, 0 Minutes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inputted entry date and time + 5 hours exactly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Input leaving date and time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Click on Calculate button</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC2</t>
   </si>
   <si>
+    <t xml:space="preserve">Valet parking – 5 hours or less – lower boundary (1 minute)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0 Days, 0 Hours, 1 Minutes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inputted entry date and time + 1 minute exactly</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC3</t>
   </si>
   <si>
+    <t xml:space="preserve">Valet parking – 5 hours or less – lower boundary less 1 minute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimated parking costs: $0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0 Days, 0 Hours, 0 Minutes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leaving date and time = Inputted entry date and time</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC4</t>
   </si>
   <si>
+    <t xml:space="preserve">Valet parking – 5 hours or less – upper boundary plus 1 minute (this is also the lower boundary of the next partition: per day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimated parking costs: $18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0 Days, 5 Hours, 1 Minutes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inputted entry date and time + 5 hours 1 minute exactly</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC5</t>
   </si>
   <si>
+    <t xml:space="preserve">Valet parking – per day – duration: 23 Hours 59 minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0 Days, 23 Hours, 59 Minutes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inputted entry date and time + 23 hours 59 minutes exactly</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC6</t>
   </si>
   <si>
+    <t xml:space="preserve">Valet parking – per day – duration: 24 Hours exactly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1 Days, 0 Hours, 0 Minutes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inputted entry date and time + 24 hours exactly</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valet parking – per day – duration: 24 Hours 1 Minute exactly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimated parking costs: $36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1 Days, 0 Hours, 1 Minutes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inputted entry date and time + 24 hours 1 minute exactly</t>
   </si>
   <si>
     <t xml:space="preserve">TC8</t>
@@ -225,47 +324,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -460,14 +559,16 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.71484375" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="47.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="54.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="56.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="47.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="7" style="1" width="47.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
@@ -494,264 +595,432 @@
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7"/>
+      <c r="B2" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="D2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="C4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
+      <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
+      <c r="D6" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="E6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="C8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="C9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
+      <c r="C10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
+      <c r="D11" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="E11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="C14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
+      <c r="C15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
+      <c r="D16" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="E16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="D17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="C18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
+      <c r="C20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="10"/>
-      <c r="D21" s="11"/>
+      <c r="D21" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="E21" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="D22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="C23" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
+      <c r="C24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
+      <c r="C25" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
       <c r="C26" s="10"/>
-      <c r="D26" s="11"/>
+      <c r="D26" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="E26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="7"/>
+        <v>36</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
+      <c r="D27" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="C28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
+      <c r="C29" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6"/>
       <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
+      <c r="C30" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6"/>
       <c r="B31" s="7"/>
       <c r="C31" s="10"/>
-      <c r="D31" s="11"/>
+      <c r="D31" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="E31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="D32" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
+      <c r="C33" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6"/>
       <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
+      <c r="C34" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
+      <c r="C35" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
       <c r="C36" s="10"/>
-      <c r="D36" s="11"/>
+      <c r="D36" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="E36" s="11"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
@@ -788,7 +1057,7 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="8"/>
@@ -825,7 +1094,7 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B47" s="7"/>
       <c r="C47" s="8"/>

</xml_diff>